<commit_message>
Highlighted more names that were corrected.
</commit_message>
<xml_diff>
--- a/SourceAssets/Active DOH 5.3.17.xlsx
+++ b/SourceAssets/Active DOH 5.3.17.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17927"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\Projects\GitHub\FaceCards\SourceAssets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jalvarado\Documents\GitHub\FaceCards\SourceAssets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24645" windowHeight="16380"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24645" windowHeight="16380" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Rows 1 to 100" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="314">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="313">
   <si>
     <t>Last Name</t>
   </si>
@@ -733,9 +733,6 @@
     <t>Leo_Simkin_Engineering.png</t>
   </si>
   <si>
-    <t>Mark_Gabby_Engineering.png</t>
-  </si>
-  <si>
     <t>Masana_Pawlan_Engineering.png</t>
   </si>
   <si>
@@ -868,9 +865,6 @@
     <t>Derek_Van Oteghem</t>
   </si>
   <si>
-    <t>Mark_Gabby-Li</t>
-  </si>
-  <si>
     <t>Matthew_Campbell</t>
   </si>
   <si>
@@ -965,6 +959,9 @@
   </si>
   <si>
     <t>Koy_Van Oteghem_Art.png</t>
+  </si>
+  <si>
+    <t>Mark_Gabby-Li_Engineering.png</t>
   </si>
 </sst>
 </file>
@@ -974,7 +971,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1007,8 +1004,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1023,6 +1027,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -1050,12 +1059,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1072,9 +1082,11 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="3"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="2" builtinId="10"/>
   </cellStyles>
@@ -1390,9 +1402,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I102"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="B139" sqref="B139"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1418,19 +1430,19 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>291</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>294</v>
-      </c>
       <c r="I1" s="1" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -3710,10 +3722,10 @@
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" s="5" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="C67" s="4">
         <v>42744</v>
@@ -4969,7 +4981,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <autoFilter ref="A1:I102"/>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4981,8 +4992,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I101"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="A62" sqref="A62"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="A99" sqref="A99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5112,7 +5123,7 @@
         <v>_Art</v>
       </c>
       <c r="E4" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F4">
         <f>MATCH(IF(ISBLANK(E4),C4, E4),'Rows 1 to 100'!D:D,0)</f>
@@ -5313,7 +5324,7 @@
         <v>_Engineering</v>
       </c>
       <c r="E10" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="F10">
         <f>MATCH(IF(ISBLANK(E10),C10, E10),'Rows 1 to 100'!D:D,0)</f>
@@ -5349,7 +5360,7 @@
         <v>_Executive</v>
       </c>
       <c r="E11" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="F11">
         <f>MATCH(IF(ISBLANK(E11),C11, E11),'Rows 1 to 100'!D:D,0)</f>
@@ -5451,7 +5462,7 @@
         <v>_Engineering</v>
       </c>
       <c r="E14" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="F14">
         <f>MATCH(IF(ISBLANK(E14),C14, E14),'Rows 1 to 100'!D:D,0)</f>
@@ -5553,7 +5564,7 @@
         <v>_Engineering</v>
       </c>
       <c r="E17" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="F17">
         <f>MATCH(IF(ISBLANK(E17),C17, E17),'Rows 1 to 100'!D:D,0)</f>
@@ -5787,7 +5798,7 @@
         <v>_Executive</v>
       </c>
       <c r="E24" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="F24">
         <f>MATCH(IF(ISBLANK(E24),C24, E24),'Rows 1 to 100'!D:D,0)</f>
@@ -5856,7 +5867,7 @@
         <v>_QA</v>
       </c>
       <c r="E26" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F26">
         <f>MATCH(IF(ISBLANK(E26),C26, E26),'Rows 1 to 100'!D:D,0)</f>
@@ -5958,7 +5969,7 @@
         <v>_Operations</v>
       </c>
       <c r="E29" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="F29">
         <f>MATCH(IF(ISBLANK(E29),C29, E29),'Rows 1 to 100'!D:D,0)</f>
@@ -6093,7 +6104,7 @@
         <v>_Engineering</v>
       </c>
       <c r="E33" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F33">
         <f>MATCH(IF(ISBLANK(E33),C33, E33),'Rows 1 to 100'!D:D,0)</f>
@@ -6178,9 +6189,9 @@
         <v>Galen_Davis</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>276</v>
+    <row r="36" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A36" s="8" t="s">
+        <v>275</v>
       </c>
       <c r="B36">
         <f t="shared" si="0"/>
@@ -6426,7 +6437,7 @@
         <v>_Art</v>
       </c>
       <c r="E43" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F43">
         <f>MATCH(IF(ISBLANK(E43),C43, E43),'Rows 1 to 100'!D:D,0)</f>
@@ -6513,7 +6524,7 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B46">
         <f t="shared" si="0"/>
@@ -6528,7 +6539,7 @@
         <v>_Engineering</v>
       </c>
       <c r="E46" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F46">
         <f>MATCH(IF(ISBLANK(E46),C46, E46),'Rows 1 to 100'!D:D,0)</f>
@@ -6714,7 +6725,7 @@
     </row>
     <row r="52" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A52" s="7" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B52">
         <f t="shared" si="0"/>
@@ -6729,7 +6740,7 @@
         <v>_Engineering</v>
       </c>
       <c r="E52" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="F52">
         <f>MATCH(IF(ISBLANK(E52),C52, E52),'Rows 1 to 100'!D:D,0)</f>
@@ -6750,7 +6761,7 @@
     </row>
     <row r="53" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A53" s="7" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="B53">
         <f t="shared" si="0"/>
@@ -6765,7 +6776,7 @@
         <v>_Art</v>
       </c>
       <c r="E53" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="F53">
         <f>MATCH(IF(ISBLANK(E53),C53, E53),'Rows 1 to 100'!D:D,0)</f>
@@ -6999,7 +7010,7 @@
         <v>_Art</v>
       </c>
       <c r="E60" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F60">
         <f>MATCH(IF(ISBLANK(E60),C60, E60),'Rows 1 to 100'!D:D,0)</f>
@@ -7053,7 +7064,7 @@
     </row>
     <row r="62" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A62" s="7" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B62">
         <f t="shared" si="0"/>
@@ -7068,7 +7079,7 @@
         <v>_Art</v>
       </c>
       <c r="E62" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F62">
         <f>MATCH(IF(ISBLANK(E62),C62, E62),'Rows 1 to 100'!D:D,0)</f>
@@ -7120,24 +7131,21 @@
         <v>Leo_Simkin</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A64" t="s">
-        <v>236</v>
+    <row r="64" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A64" s="7" t="s">
+        <v>312</v>
       </c>
       <c r="B64">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C64" t="str">
         <f t="shared" si="1"/>
-        <v>Mark_Gabby</v>
+        <v>Mark_Gabby-Li</v>
       </c>
       <c r="D64" t="str">
         <f t="shared" si="2"/>
         <v>_Engineering</v>
-      </c>
-      <c r="E64" t="s">
-        <v>281</v>
       </c>
       <c r="F64">
         <f>MATCH(IF(ISBLANK(E64),C64, E64),'Rows 1 to 100'!D:D,0)</f>
@@ -7145,11 +7153,11 @@
       </c>
       <c r="G64" t="str">
         <f ca="1">C64&amp;D64&amp;"_"&amp;OFFSET('Rows 1 to 100'!$H$1,F64-1,0)</f>
-        <v>Mark_Gabby_Engineering_2015-07-06</v>
+        <v>Mark_Gabby-Li_Engineering_2015-07-06</v>
       </c>
       <c r="H64" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>rename "Mark_Gabby_Engineering.png" "Mark_Gabby_Engineering_2015-07-06.png"</v>
+        <v>rename "Mark_Gabby-Li_Engineering.png" "Mark_Gabby-Li_Engineering_2015-07-06.png"</v>
       </c>
       <c r="I64" t="str">
         <f t="shared" si="4"/>
@@ -7158,7 +7166,7 @@
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B65">
         <f t="shared" si="0"/>
@@ -7191,7 +7199,7 @@
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B66">
         <f t="shared" ref="B66:B101" si="5">FIND("_",A66,FIND("_",A66)+1)</f>
@@ -7224,7 +7232,7 @@
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B67">
         <f t="shared" si="5"/>
@@ -7239,7 +7247,7 @@
         <v>_Engineering</v>
       </c>
       <c r="E67" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F67">
         <f>MATCH(IF(ISBLANK(E67),C67, E67),'Rows 1 to 100'!D:D,0)</f>
@@ -7260,7 +7268,7 @@
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B68">
         <f t="shared" si="5"/>
@@ -7275,7 +7283,7 @@
         <v>_Production</v>
       </c>
       <c r="E68" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="F68">
         <f>MATCH(IF(ISBLANK(E68),C68, E68),'Rows 1 to 100'!D:D,0)</f>
@@ -7296,7 +7304,7 @@
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B69">
         <f t="shared" si="5"/>
@@ -7329,7 +7337,7 @@
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B70">
         <f t="shared" si="5"/>
@@ -7344,7 +7352,7 @@
         <v>_Production</v>
       </c>
       <c r="E70" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="F70">
         <f>MATCH(IF(ISBLANK(E70),C70, E70),'Rows 1 to 100'!D:D,0)</f>
@@ -7365,7 +7373,7 @@
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B71">
         <f t="shared" si="5"/>
@@ -7380,7 +7388,7 @@
         <v>_Engineering</v>
       </c>
       <c r="E71" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="F71">
         <f>MATCH(IF(ISBLANK(E71),C71, E71),'Rows 1 to 100'!D:D,0)</f>
@@ -7401,7 +7409,7 @@
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B72">
         <f t="shared" si="5"/>
@@ -7434,7 +7442,7 @@
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B73">
         <f t="shared" si="5"/>
@@ -7449,7 +7457,7 @@
         <v>_Engineering</v>
       </c>
       <c r="E73" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="F73">
         <f>MATCH(IF(ISBLANK(E73),C73, E73),'Rows 1 to 100'!D:D,0)</f>
@@ -7470,7 +7478,7 @@
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B74">
         <f t="shared" si="5"/>
@@ -7503,7 +7511,7 @@
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B75">
         <f t="shared" si="5"/>
@@ -7518,7 +7526,7 @@
         <v>_Engineering</v>
       </c>
       <c r="E75" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="F75">
         <f>MATCH(IF(ISBLANK(E75),C75, E75),'Rows 1 to 100'!D:D,0)</f>
@@ -7539,7 +7547,7 @@
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B76">
         <f t="shared" si="5"/>
@@ -7572,7 +7580,7 @@
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B77">
         <f t="shared" si="5"/>
@@ -7605,7 +7613,7 @@
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B78">
         <f t="shared" si="5"/>
@@ -7638,7 +7646,7 @@
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B79">
         <f t="shared" si="5"/>
@@ -7671,7 +7679,7 @@
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B80">
         <f t="shared" si="5"/>
@@ -7686,7 +7694,7 @@
         <v>_Art</v>
       </c>
       <c r="E80" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="F80">
         <f>MATCH(IF(ISBLANK(E80),C80, E80),'Rows 1 to 100'!D:D,0)</f>
@@ -7707,7 +7715,7 @@
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B81">
         <f t="shared" si="5"/>
@@ -7722,7 +7730,7 @@
         <v>_IT-QA</v>
       </c>
       <c r="E81" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F81">
         <f>MATCH(IF(ISBLANK(E81),C81, E81),'Rows 1 to 100'!D:D,0)</f>
@@ -7743,7 +7751,7 @@
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B82">
         <f t="shared" si="5"/>
@@ -7776,7 +7784,7 @@
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B83">
         <f t="shared" si="5"/>
@@ -7809,7 +7817,7 @@
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B84">
         <f t="shared" si="5"/>
@@ -7842,7 +7850,7 @@
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B85">
         <f t="shared" si="5"/>
@@ -7875,7 +7883,7 @@
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B86">
         <f t="shared" si="5"/>
@@ -7908,7 +7916,7 @@
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B87">
         <f t="shared" si="5"/>
@@ -7941,7 +7949,7 @@
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B88">
         <f t="shared" si="5"/>
@@ -7974,7 +7982,7 @@
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B89">
         <f t="shared" si="5"/>
@@ -8007,7 +8015,7 @@
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B90">
         <f t="shared" si="5"/>
@@ -8040,7 +8048,7 @@
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B91">
         <f t="shared" si="5"/>
@@ -8073,7 +8081,7 @@
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B92">
         <f t="shared" si="5"/>
@@ -8106,7 +8114,7 @@
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B93">
         <f t="shared" si="5"/>
@@ -8121,7 +8129,7 @@
         <v>_Art</v>
       </c>
       <c r="E93" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="F93">
         <f>MATCH(IF(ISBLANK(E93),C93, E93),'Rows 1 to 100'!D:D,0)</f>
@@ -8142,7 +8150,7 @@
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B94">
         <f t="shared" si="5"/>
@@ -8175,7 +8183,7 @@
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A95" s="6" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B95">
         <f t="shared" si="5"/>
@@ -8208,7 +8216,7 @@
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A96" s="6" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B96">
         <f t="shared" si="5"/>
@@ -8241,7 +8249,7 @@
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A97" s="6" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B97">
         <f t="shared" si="5"/>
@@ -8256,7 +8264,7 @@
         <v>_QA</v>
       </c>
       <c r="E97" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="F97">
         <f>MATCH(IF(ISBLANK(E97),C97, E97),'Rows 1 to 100'!D:D,0)</f>
@@ -8277,7 +8285,7 @@
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A98" s="6" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B98">
         <f t="shared" si="5"/>
@@ -8310,7 +8318,7 @@
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A99" s="6" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="B99">
         <f t="shared" si="5"/>
@@ -8325,7 +8333,7 @@
         <v>_Production</v>
       </c>
       <c r="E99" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="F99">
         <f>MATCH(IF(ISBLANK(E99),C99, E99),'Rows 1 to 100'!D:D,0)</f>
@@ -8346,7 +8354,7 @@
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A100" s="6" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="B100">
         <f t="shared" si="5"/>
@@ -8379,7 +8387,7 @@
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A101" s="6" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B101">
         <f t="shared" si="5"/>
@@ -8394,7 +8402,7 @@
         <v>_Art</v>
       </c>
       <c r="E101" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="F101">
         <f>MATCH(IF(ISBLANK(E101),C101, E101),'Rows 1 to 100'!D:D,0)</f>
@@ -8414,7 +8422,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>